<commit_message>
Added more to report
</commit_message>
<xml_diff>
--- a/Study Results.xlsx
+++ b/Study Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Louis\Desktop\CS\2296038-final-year-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B956924C-7432-41A4-8D7B-51E3C83FFB1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22B5CCFA-EDC7-41BD-9DCF-255209BEF015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Data" sheetId="1" r:id="rId1"/>
@@ -381,24 +381,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00FF00"/>
-        <bgColor rgb="FF00FF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FFFF0000"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -413,14 +401,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -701,10 +687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AN20"/>
+  <dimension ref="A1:AN25"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AG30" sqref="AG30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2808,25 +2794,994 @@
         <v>5</v>
       </c>
     </row>
+    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18">
+        <v>4</v>
+      </c>
+      <c r="F18">
+        <v>4</v>
+      </c>
+      <c r="G18">
+        <v>4</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>5</v>
+      </c>
+      <c r="K18">
+        <v>4</v>
+      </c>
+      <c r="L18">
+        <v>3</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <v>1</v>
+      </c>
+      <c r="P18">
+        <v>4</v>
+      </c>
+      <c r="Q18">
+        <v>4</v>
+      </c>
+      <c r="R18">
+        <v>5</v>
+      </c>
+      <c r="S18">
+        <v>5</v>
+      </c>
+      <c r="T18">
+        <v>4</v>
+      </c>
+      <c r="U18">
+        <v>4</v>
+      </c>
+      <c r="V18">
+        <v>4</v>
+      </c>
+      <c r="W18">
+        <v>4</v>
+      </c>
+      <c r="X18">
+        <v>4</v>
+      </c>
+      <c r="Y18">
+        <v>1</v>
+      </c>
+      <c r="Z18">
+        <v>1</v>
+      </c>
+      <c r="AA18">
+        <v>1</v>
+      </c>
+      <c r="AB18">
+        <v>1</v>
+      </c>
+      <c r="AC18">
+        <v>0</v>
+      </c>
+      <c r="AD18">
+        <v>6</v>
+      </c>
+      <c r="AE18">
+        <v>5</v>
+      </c>
+      <c r="AF18">
+        <v>4</v>
+      </c>
+      <c r="AG18">
+        <v>1</v>
+      </c>
+      <c r="AH18">
+        <v>5</v>
+      </c>
+      <c r="AI18">
+        <v>1</v>
+      </c>
+      <c r="AJ18">
+        <v>9</v>
+      </c>
+      <c r="AK18">
+        <v>5</v>
+      </c>
+      <c r="AL18">
+        <v>5</v>
+      </c>
+      <c r="AM18">
+        <v>1</v>
+      </c>
+      <c r="AN18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+      <c r="E19">
+        <v>4</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="G19">
+        <v>3</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>5</v>
+      </c>
+      <c r="J19">
+        <v>4</v>
+      </c>
+      <c r="K19">
+        <v>5</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>4</v>
+      </c>
+      <c r="O19">
+        <v>2</v>
+      </c>
+      <c r="P19">
+        <v>5</v>
+      </c>
+      <c r="Q19">
+        <v>5</v>
+      </c>
+      <c r="R19">
+        <v>5</v>
+      </c>
+      <c r="S19">
+        <v>4</v>
+      </c>
+      <c r="T19">
+        <v>5</v>
+      </c>
+      <c r="U19">
+        <v>4</v>
+      </c>
+      <c r="V19">
+        <v>4</v>
+      </c>
+      <c r="W19">
+        <v>2</v>
+      </c>
+      <c r="X19">
+        <v>4</v>
+      </c>
+      <c r="Y19">
+        <v>4</v>
+      </c>
+      <c r="Z19">
+        <v>4</v>
+      </c>
+      <c r="AA19">
+        <v>4</v>
+      </c>
+      <c r="AB19">
+        <v>4</v>
+      </c>
+      <c r="AC19">
+        <v>0</v>
+      </c>
+      <c r="AD19">
+        <v>4</v>
+      </c>
+      <c r="AE19">
+        <v>4</v>
+      </c>
+      <c r="AF19">
+        <v>2</v>
+      </c>
+      <c r="AG19">
+        <v>1</v>
+      </c>
+      <c r="AH19">
+        <v>4</v>
+      </c>
+      <c r="AI19">
+        <v>1</v>
+      </c>
+      <c r="AJ19">
+        <v>0</v>
+      </c>
+      <c r="AK19">
+        <v>4</v>
+      </c>
+      <c r="AL19">
+        <v>3</v>
+      </c>
+      <c r="AM19">
+        <v>1</v>
+      </c>
+      <c r="AN19">
+        <v>4</v>
+      </c>
+    </row>
     <row r="20" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20">
+        <v>3</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+      <c r="G20">
+        <v>4</v>
+      </c>
+      <c r="H20">
+        <v>2</v>
+      </c>
+      <c r="I20">
+        <v>2</v>
+      </c>
+      <c r="J20">
+        <v>2</v>
+      </c>
+      <c r="K20">
+        <v>4</v>
+      </c>
+      <c r="L20">
+        <v>3</v>
+      </c>
+      <c r="M20">
+        <v>4</v>
+      </c>
+      <c r="N20">
+        <v>2</v>
+      </c>
+      <c r="O20">
+        <v>2</v>
+      </c>
+      <c r="P20">
+        <v>4</v>
+      </c>
+      <c r="Q20">
+        <v>2</v>
+      </c>
+      <c r="R20">
+        <v>5</v>
+      </c>
+      <c r="S20">
+        <v>5</v>
+      </c>
+      <c r="T20">
+        <v>5</v>
+      </c>
+      <c r="U20">
+        <v>5</v>
+      </c>
+      <c r="V20">
+        <v>5</v>
+      </c>
+      <c r="W20">
+        <v>4</v>
+      </c>
+      <c r="X20">
+        <v>4</v>
+      </c>
+      <c r="Y20">
+        <v>3</v>
+      </c>
+      <c r="Z20">
+        <v>3</v>
+      </c>
+      <c r="AA20">
+        <v>3</v>
+      </c>
+      <c r="AB20">
+        <v>4</v>
+      </c>
+      <c r="AC20">
+        <v>1</v>
+      </c>
+      <c r="AD20">
+        <v>5</v>
+      </c>
+      <c r="AE20">
+        <v>4</v>
+      </c>
+      <c r="AF20">
+        <v>2</v>
+      </c>
+      <c r="AG20">
+        <v>1</v>
+      </c>
+      <c r="AH20">
+        <v>4</v>
+      </c>
+      <c r="AI20">
+        <v>0</v>
+      </c>
+      <c r="AJ20">
+        <v>6</v>
+      </c>
+      <c r="AK20">
+        <v>5</v>
+      </c>
+      <c r="AL20">
+        <v>4</v>
+      </c>
+      <c r="AM20">
+        <v>1</v>
+      </c>
+      <c r="AN20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>4</v>
+      </c>
+      <c r="E21">
+        <v>3</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>2</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>4</v>
+      </c>
+      <c r="J21">
+        <v>4</v>
+      </c>
+      <c r="K21">
+        <v>5</v>
+      </c>
+      <c r="L21">
+        <v>4</v>
+      </c>
+      <c r="M21">
+        <v>4</v>
+      </c>
+      <c r="N21">
+        <v>2</v>
+      </c>
+      <c r="O21">
+        <v>4</v>
+      </c>
+      <c r="P21">
+        <v>4</v>
+      </c>
+      <c r="Q21">
+        <v>2</v>
+      </c>
+      <c r="R21">
+        <v>5</v>
+      </c>
+      <c r="S21">
+        <v>2</v>
+      </c>
+      <c r="T21">
+        <v>2</v>
+      </c>
+      <c r="U21">
+        <v>2</v>
+      </c>
+      <c r="V21">
+        <v>4</v>
+      </c>
+      <c r="W21">
+        <v>4</v>
+      </c>
+      <c r="X21">
+        <v>4</v>
+      </c>
+      <c r="Y21">
+        <v>2</v>
+      </c>
+      <c r="Z21">
+        <v>1</v>
+      </c>
+      <c r="AA21">
+        <v>2</v>
+      </c>
+      <c r="AB21">
+        <v>2</v>
+      </c>
+      <c r="AC21">
+        <v>0</v>
+      </c>
+      <c r="AD21">
+        <v>8</v>
+      </c>
+      <c r="AE21">
+        <v>4</v>
+      </c>
+      <c r="AF21">
+        <v>4</v>
+      </c>
+      <c r="AG21">
+        <v>1</v>
+      </c>
+      <c r="AH21">
+        <v>5</v>
+      </c>
+      <c r="AI21">
+        <v>1</v>
+      </c>
+      <c r="AJ21">
+        <v>7</v>
+      </c>
+      <c r="AK21">
+        <v>4</v>
+      </c>
+      <c r="AL21">
+        <v>4</v>
+      </c>
+      <c r="AM21">
+        <v>1</v>
+      </c>
+      <c r="AN21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>5</v>
+      </c>
+      <c r="E22">
+        <v>4</v>
+      </c>
+      <c r="F22">
+        <v>4</v>
+      </c>
+      <c r="G22">
+        <v>3</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>2</v>
+      </c>
+      <c r="J22">
+        <v>4</v>
+      </c>
+      <c r="K22">
+        <v>3</v>
+      </c>
+      <c r="L22">
+        <v>3</v>
+      </c>
+      <c r="M22">
+        <v>2</v>
+      </c>
+      <c r="N22">
+        <v>4</v>
+      </c>
+      <c r="O22">
+        <v>1</v>
+      </c>
+      <c r="P22">
+        <v>3</v>
+      </c>
+      <c r="Q22">
+        <v>2</v>
+      </c>
+      <c r="R22">
+        <v>4</v>
+      </c>
+      <c r="S22">
+        <v>4</v>
+      </c>
+      <c r="T22">
+        <v>4</v>
+      </c>
+      <c r="U22">
+        <v>5</v>
+      </c>
+      <c r="V22">
+        <v>5</v>
+      </c>
+      <c r="W22">
+        <v>5</v>
+      </c>
+      <c r="X22">
+        <v>5</v>
+      </c>
+      <c r="Y22">
+        <v>3</v>
+      </c>
+      <c r="Z22">
+        <v>2</v>
+      </c>
+      <c r="AA22">
+        <v>2</v>
+      </c>
+      <c r="AB22">
+        <v>5</v>
+      </c>
+      <c r="AC22">
+        <v>0</v>
+      </c>
+      <c r="AD22">
+        <v>10</v>
+      </c>
+      <c r="AE22">
+        <v>4</v>
+      </c>
+      <c r="AF22">
+        <v>4</v>
+      </c>
+      <c r="AG22">
+        <v>1</v>
+      </c>
+      <c r="AH22">
+        <v>4</v>
+      </c>
+      <c r="AI22">
+        <v>1</v>
+      </c>
+      <c r="AJ22">
+        <v>10</v>
+      </c>
+      <c r="AK22">
+        <v>5</v>
+      </c>
+      <c r="AL22">
+        <v>5</v>
+      </c>
+      <c r="AM22">
+        <v>2</v>
+      </c>
+      <c r="AN22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>5</v>
+      </c>
+      <c r="D23">
+        <v>4</v>
+      </c>
+      <c r="E23">
+        <v>3</v>
+      </c>
+      <c r="F23">
+        <v>4</v>
+      </c>
+      <c r="G23">
+        <v>5</v>
+      </c>
+      <c r="H23">
+        <v>2</v>
+      </c>
+      <c r="I23">
+        <v>5</v>
+      </c>
+      <c r="J23">
+        <v>5</v>
+      </c>
+      <c r="K23">
+        <v>4</v>
+      </c>
+      <c r="L23">
+        <v>2</v>
+      </c>
+      <c r="M23">
+        <v>2</v>
+      </c>
+      <c r="N23">
+        <v>2</v>
+      </c>
+      <c r="O23">
+        <v>2</v>
+      </c>
+      <c r="P23">
+        <v>4</v>
+      </c>
+      <c r="Q23">
+        <v>4</v>
+      </c>
+      <c r="R23">
+        <v>4</v>
+      </c>
+      <c r="S23">
+        <v>4</v>
+      </c>
+      <c r="T23">
+        <v>4</v>
+      </c>
+      <c r="U23">
+        <v>4</v>
+      </c>
+      <c r="V23">
+        <v>4</v>
+      </c>
+      <c r="W23">
+        <v>3</v>
+      </c>
+      <c r="X23">
+        <v>4</v>
+      </c>
+      <c r="Y23">
+        <v>4</v>
+      </c>
+      <c r="Z23">
+        <v>4</v>
+      </c>
+      <c r="AA23">
+        <v>3</v>
+      </c>
+      <c r="AB23">
+        <v>4</v>
+      </c>
+      <c r="AC23">
+        <v>0</v>
+      </c>
+      <c r="AD23">
+        <v>5</v>
+      </c>
+      <c r="AE23">
+        <v>5</v>
+      </c>
+      <c r="AF23">
+        <v>4</v>
+      </c>
+      <c r="AG23">
+        <v>1</v>
+      </c>
+      <c r="AH23">
+        <v>5</v>
+      </c>
+      <c r="AI23">
+        <v>1</v>
+      </c>
+      <c r="AJ23">
+        <v>5</v>
+      </c>
+      <c r="AK23">
+        <v>4</v>
+      </c>
+      <c r="AL23">
+        <v>4</v>
+      </c>
+      <c r="AM23">
+        <v>1</v>
+      </c>
+      <c r="AN23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>5</v>
+      </c>
+      <c r="E24">
+        <v>3</v>
+      </c>
+      <c r="F24">
+        <v>4</v>
+      </c>
+      <c r="G24">
+        <v>3</v>
+      </c>
+      <c r="H24">
+        <v>2</v>
+      </c>
+      <c r="I24">
+        <v>4</v>
+      </c>
+      <c r="J24">
+        <v>3</v>
+      </c>
+      <c r="K24">
+        <v>3</v>
+      </c>
+      <c r="L24">
+        <v>2</v>
+      </c>
+      <c r="M24">
+        <v>4</v>
+      </c>
+      <c r="N24">
+        <v>1</v>
+      </c>
+      <c r="O24">
+        <v>3</v>
+      </c>
+      <c r="P24">
+        <v>2</v>
+      </c>
+      <c r="Q24">
+        <v>4</v>
+      </c>
+      <c r="R24">
+        <v>4</v>
+      </c>
+      <c r="S24">
+        <v>3</v>
+      </c>
+      <c r="T24">
+        <v>4</v>
+      </c>
+      <c r="U24">
+        <v>4</v>
+      </c>
+      <c r="V24">
+        <v>5</v>
+      </c>
+      <c r="W24">
+        <v>4</v>
+      </c>
+      <c r="X24">
+        <v>3</v>
+      </c>
+      <c r="Y24">
+        <v>3</v>
+      </c>
+      <c r="Z24">
+        <v>3</v>
+      </c>
+      <c r="AA24">
+        <v>3</v>
+      </c>
+      <c r="AB24">
+        <v>4</v>
+      </c>
+      <c r="AC24">
+        <v>1</v>
+      </c>
+      <c r="AD24">
+        <v>6</v>
+      </c>
+      <c r="AE24">
+        <v>4</v>
+      </c>
+      <c r="AF24">
+        <v>4</v>
+      </c>
+      <c r="AG24">
+        <v>1</v>
+      </c>
+      <c r="AH24">
+        <v>5</v>
+      </c>
+      <c r="AI24">
+        <v>0</v>
+      </c>
+      <c r="AJ24">
+        <v>5</v>
+      </c>
+      <c r="AK24">
+        <v>4</v>
+      </c>
+      <c r="AL24">
+        <v>5</v>
+      </c>
+      <c r="AM24">
+        <v>1</v>
+      </c>
+      <c r="AN24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25">
+        <v>5</v>
+      </c>
+      <c r="E25">
+        <v>3</v>
+      </c>
+      <c r="F25">
+        <v>2</v>
+      </c>
+      <c r="G25">
+        <v>2</v>
+      </c>
+      <c r="H25">
+        <v>4</v>
+      </c>
+      <c r="I25">
+        <v>4</v>
+      </c>
+      <c r="J25">
+        <v>4</v>
+      </c>
+      <c r="K25">
+        <v>3</v>
+      </c>
+      <c r="L25">
+        <v>4</v>
+      </c>
+      <c r="M25">
+        <v>5</v>
+      </c>
+      <c r="N25">
+        <v>3</v>
+      </c>
+      <c r="O25">
+        <v>2</v>
+      </c>
+      <c r="P25">
+        <v>3</v>
+      </c>
+      <c r="Q25">
+        <v>2</v>
+      </c>
+      <c r="R25">
+        <v>5</v>
+      </c>
+      <c r="S25">
+        <v>4</v>
+      </c>
+      <c r="T25">
+        <v>4</v>
+      </c>
+      <c r="U25">
+        <v>5</v>
+      </c>
+      <c r="V25">
+        <v>5</v>
+      </c>
+      <c r="W25">
+        <v>4</v>
+      </c>
+      <c r="X25">
+        <v>4</v>
+      </c>
+      <c r="Y25">
+        <v>2</v>
+      </c>
+      <c r="Z25">
+        <v>2</v>
+      </c>
+      <c r="AA25">
+        <v>2</v>
+      </c>
+      <c r="AB25">
+        <v>4</v>
+      </c>
+      <c r="AC25">
+        <v>0</v>
+      </c>
+      <c r="AD25">
+        <v>5</v>
+      </c>
+      <c r="AE25">
+        <v>5</v>
+      </c>
+      <c r="AF25">
+        <v>4</v>
+      </c>
+      <c r="AG25">
+        <v>1</v>
+      </c>
+      <c r="AH25">
+        <v>5</v>
+      </c>
+      <c r="AI25">
+        <v>1</v>
+      </c>
+      <c r="AJ25">
+        <v>4</v>
+      </c>
+      <c r="AK25">
+        <v>4</v>
+      </c>
+      <c r="AL25">
+        <v>4</v>
+      </c>
+      <c r="AM25">
+        <v>4</v>
+      </c>
+      <c r="AN25">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:W17"/>
+  <dimension ref="A1:W1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="W14" sqref="W14"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="R30" sqref="R30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2915,1142 +3870,6 @@
       </c>
       <c r="W1" s="1" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>4</v>
-      </c>
-      <c r="E2">
-        <v>4</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>6</v>
-      </c>
-      <c r="H2">
-        <v>-4</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>9</v>
-      </c>
-      <c r="K2">
-        <v>17</v>
-      </c>
-      <c r="L2">
-        <v>6</v>
-      </c>
-      <c r="M2">
-        <v>5</v>
-      </c>
-      <c r="N2">
-        <v>5</v>
-      </c>
-      <c r="O2">
-        <v>4</v>
-      </c>
-      <c r="P2">
-        <v>2</v>
-      </c>
-      <c r="Q2">
-        <v>4</v>
-      </c>
-      <c r="R2">
-        <v>6</v>
-      </c>
-      <c r="S2">
-        <v>3</v>
-      </c>
-      <c r="T2">
-        <v>5</v>
-      </c>
-      <c r="U2">
-        <v>4</v>
-      </c>
-      <c r="V2">
-        <v>4</v>
-      </c>
-      <c r="W2" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>4</v>
-      </c>
-      <c r="E3">
-        <v>4</v>
-      </c>
-      <c r="F3">
-        <v>-2</v>
-      </c>
-      <c r="G3">
-        <v>7</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>8</v>
-      </c>
-      <c r="J3">
-        <v>7</v>
-      </c>
-      <c r="K3">
-        <v>19</v>
-      </c>
-      <c r="L3">
-        <v>6</v>
-      </c>
-      <c r="M3">
-        <v>3</v>
-      </c>
-      <c r="N3">
-        <v>5</v>
-      </c>
-      <c r="O3">
-        <v>5</v>
-      </c>
-      <c r="P3">
-        <v>1</v>
-      </c>
-      <c r="Q3">
-        <v>5</v>
-      </c>
-      <c r="R3">
-        <v>4</v>
-      </c>
-      <c r="S3">
-        <v>4</v>
-      </c>
-      <c r="T3">
-        <v>5</v>
-      </c>
-      <c r="U3">
-        <v>1</v>
-      </c>
-      <c r="V3">
-        <v>4</v>
-      </c>
-      <c r="W3" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>6</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
-      <c r="G4">
-        <v>5</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>2</v>
-      </c>
-      <c r="J4">
-        <v>6</v>
-      </c>
-      <c r="K4">
-        <v>14</v>
-      </c>
-      <c r="L4">
-        <v>14</v>
-      </c>
-      <c r="M4">
-        <v>4</v>
-      </c>
-      <c r="N4">
-        <v>5</v>
-      </c>
-      <c r="O4">
-        <v>4</v>
-      </c>
-      <c r="P4">
-        <v>1</v>
-      </c>
-      <c r="Q4">
-        <v>4</v>
-      </c>
-      <c r="R4">
-        <v>6</v>
-      </c>
-      <c r="S4">
-        <v>3</v>
-      </c>
-      <c r="T4">
-        <v>5</v>
-      </c>
-      <c r="U4">
-        <v>4</v>
-      </c>
-      <c r="V4">
-        <v>4</v>
-      </c>
-      <c r="W4" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-      <c r="E5">
-        <v>3</v>
-      </c>
-      <c r="F5">
-        <v>5</v>
-      </c>
-      <c r="G5">
-        <v>3</v>
-      </c>
-      <c r="H5">
-        <v>-4</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>6</v>
-      </c>
-      <c r="K5">
-        <v>20</v>
-      </c>
-      <c r="L5">
-        <v>9</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <v>5</v>
-      </c>
-      <c r="O5">
-        <v>4</v>
-      </c>
-      <c r="P5">
-        <v>2</v>
-      </c>
-      <c r="Q5">
-        <v>4</v>
-      </c>
-      <c r="R5">
-        <v>10</v>
-      </c>
-      <c r="S5">
-        <v>5</v>
-      </c>
-      <c r="T5">
-        <v>4</v>
-      </c>
-      <c r="U5">
-        <v>2</v>
-      </c>
-      <c r="V5">
-        <v>4</v>
-      </c>
-      <c r="W5" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>6</v>
-      </c>
-      <c r="D6">
-        <v>3</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>4</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>2</v>
-      </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
-      <c r="K6">
-        <v>10</v>
-      </c>
-      <c r="L6">
-        <v>15</v>
-      </c>
-      <c r="M6">
-        <v>5</v>
-      </c>
-      <c r="N6">
-        <v>5</v>
-      </c>
-      <c r="O6">
-        <v>3</v>
-      </c>
-      <c r="P6">
-        <v>2</v>
-      </c>
-      <c r="Q6">
-        <v>3</v>
-      </c>
-      <c r="R6">
-        <v>4</v>
-      </c>
-      <c r="S6">
-        <v>2</v>
-      </c>
-      <c r="T6">
-        <v>2</v>
-      </c>
-      <c r="U6">
-        <v>3</v>
-      </c>
-      <c r="V6">
-        <v>2</v>
-      </c>
-      <c r="W6" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>4</v>
-      </c>
-      <c r="E7">
-        <v>3</v>
-      </c>
-      <c r="F7">
-        <v>2</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>-5</v>
-      </c>
-      <c r="I7">
-        <v>3</v>
-      </c>
-      <c r="J7">
-        <v>-1</v>
-      </c>
-      <c r="K7">
-        <v>16</v>
-      </c>
-      <c r="L7">
-        <v>5</v>
-      </c>
-      <c r="M7">
-        <v>5</v>
-      </c>
-      <c r="N7">
-        <v>4</v>
-      </c>
-      <c r="O7">
-        <v>1</v>
-      </c>
-      <c r="P7">
-        <v>1</v>
-      </c>
-      <c r="Q7">
-        <v>2</v>
-      </c>
-      <c r="R7">
-        <v>7</v>
-      </c>
-      <c r="S7">
-        <v>4</v>
-      </c>
-      <c r="T7">
-        <v>5</v>
-      </c>
-      <c r="U7">
-        <v>3</v>
-      </c>
-      <c r="V7">
-        <v>3</v>
-      </c>
-      <c r="W7" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8">
-        <v>4</v>
-      </c>
-      <c r="E8">
-        <v>3</v>
-      </c>
-      <c r="F8">
-        <v>8</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8">
-        <v>2</v>
-      </c>
-      <c r="I8">
-        <v>3</v>
-      </c>
-      <c r="J8">
-        <v>2</v>
-      </c>
-      <c r="K8">
-        <v>14</v>
-      </c>
-      <c r="L8">
-        <v>14</v>
-      </c>
-      <c r="M8">
-        <v>4</v>
-      </c>
-      <c r="N8">
-        <v>5</v>
-      </c>
-      <c r="O8">
-        <v>4</v>
-      </c>
-      <c r="P8">
-        <v>1</v>
-      </c>
-      <c r="Q8">
-        <v>4</v>
-      </c>
-      <c r="R8">
-        <v>6</v>
-      </c>
-      <c r="S8">
-        <v>1</v>
-      </c>
-      <c r="T8">
-        <v>5</v>
-      </c>
-      <c r="U8">
-        <v>4</v>
-      </c>
-      <c r="V8">
-        <v>2</v>
-      </c>
-      <c r="W8" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>4</v>
-      </c>
-      <c r="E9">
-        <v>3</v>
-      </c>
-      <c r="F9">
-        <v>5</v>
-      </c>
-      <c r="G9">
-        <v>3</v>
-      </c>
-      <c r="H9">
-        <v>-5</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-      <c r="J9">
-        <v>5</v>
-      </c>
-      <c r="K9">
-        <v>20</v>
-      </c>
-      <c r="L9">
-        <v>9</v>
-      </c>
-      <c r="M9">
-        <v>5</v>
-      </c>
-      <c r="N9">
-        <v>4</v>
-      </c>
-      <c r="O9">
-        <v>4</v>
-      </c>
-      <c r="P9">
-        <v>1</v>
-      </c>
-      <c r="Q9">
-        <v>4</v>
-      </c>
-      <c r="R9">
-        <v>6</v>
-      </c>
-      <c r="S9">
-        <v>5</v>
-      </c>
-      <c r="T9">
-        <v>4</v>
-      </c>
-      <c r="U9">
-        <v>2</v>
-      </c>
-      <c r="V9">
-        <v>4</v>
-      </c>
-      <c r="W9" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>5</v>
-      </c>
-      <c r="D10">
-        <v>4</v>
-      </c>
-      <c r="E10">
-        <v>4</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10">
-        <v>4</v>
-      </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
-      <c r="I10">
-        <v>6</v>
-      </c>
-      <c r="J10">
-        <v>5</v>
-      </c>
-      <c r="K10">
-        <v>17</v>
-      </c>
-      <c r="L10">
-        <v>9</v>
-      </c>
-      <c r="M10">
-        <v>10</v>
-      </c>
-      <c r="N10">
-        <v>4</v>
-      </c>
-      <c r="O10">
-        <v>5</v>
-      </c>
-      <c r="P10">
-        <v>1</v>
-      </c>
-      <c r="Q10">
-        <v>4</v>
-      </c>
-      <c r="R10">
-        <v>10</v>
-      </c>
-      <c r="S10">
-        <v>4</v>
-      </c>
-      <c r="T10">
-        <v>4</v>
-      </c>
-      <c r="U10">
-        <v>2</v>
-      </c>
-      <c r="V10">
-        <v>4</v>
-      </c>
-      <c r="W10" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
-      <c r="C11">
-        <v>5</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>2</v>
-      </c>
-      <c r="F11">
-        <v>5</v>
-      </c>
-      <c r="G11">
-        <v>7</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>2</v>
-      </c>
-      <c r="J11">
-        <v>3</v>
-      </c>
-      <c r="K11">
-        <v>16</v>
-      </c>
-      <c r="L11">
-        <v>13</v>
-      </c>
-      <c r="M11">
-        <v>8</v>
-      </c>
-      <c r="N11">
-        <v>4</v>
-      </c>
-      <c r="O11">
-        <v>4</v>
-      </c>
-      <c r="P11">
-        <v>4</v>
-      </c>
-      <c r="Q11">
-        <v>4</v>
-      </c>
-      <c r="R11">
-        <v>0</v>
-      </c>
-      <c r="S11">
-        <v>4</v>
-      </c>
-      <c r="T11">
-        <v>4</v>
-      </c>
-      <c r="U11">
-        <v>4</v>
-      </c>
-      <c r="V11">
-        <v>4</v>
-      </c>
-      <c r="W11" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>2</v>
-      </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="D12">
-        <v>5</v>
-      </c>
-      <c r="E12">
-        <v>3</v>
-      </c>
-      <c r="F12">
-        <v>-2</v>
-      </c>
-      <c r="G12">
-        <v>2</v>
-      </c>
-      <c r="H12">
-        <v>-1</v>
-      </c>
-      <c r="I12">
-        <v>8</v>
-      </c>
-      <c r="J12">
-        <v>2</v>
-      </c>
-      <c r="K12">
-        <v>15</v>
-      </c>
-      <c r="L12">
-        <v>9</v>
-      </c>
-      <c r="M12">
-        <v>10</v>
-      </c>
-      <c r="N12">
-        <v>5</v>
-      </c>
-      <c r="O12">
-        <v>4</v>
-      </c>
-      <c r="P12">
-        <v>2</v>
-      </c>
-      <c r="Q12">
-        <v>4</v>
-      </c>
-      <c r="R12">
-        <v>2</v>
-      </c>
-      <c r="S12">
-        <v>4</v>
-      </c>
-      <c r="T12">
-        <v>4</v>
-      </c>
-      <c r="U12">
-        <v>2</v>
-      </c>
-      <c r="V12">
-        <v>4</v>
-      </c>
-      <c r="W12" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>4</v>
-      </c>
-      <c r="D13">
-        <v>4</v>
-      </c>
-      <c r="E13">
-        <v>5</v>
-      </c>
-      <c r="F13">
-        <v>-1</v>
-      </c>
-      <c r="G13">
-        <v>6</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>3</v>
-      </c>
-      <c r="J13">
-        <v>5</v>
-      </c>
-      <c r="K13">
-        <v>14</v>
-      </c>
-      <c r="L13">
-        <v>10</v>
-      </c>
-      <c r="M13">
-        <v>5</v>
-      </c>
-      <c r="N13">
-        <v>5</v>
-      </c>
-      <c r="O13">
-        <v>4</v>
-      </c>
-      <c r="P13">
-        <v>2</v>
-      </c>
-      <c r="Q13">
-        <v>4</v>
-      </c>
-      <c r="R13">
-        <v>4</v>
-      </c>
-      <c r="S13">
-        <v>5</v>
-      </c>
-      <c r="T13">
-        <v>5</v>
-      </c>
-      <c r="U13">
-        <v>3</v>
-      </c>
-      <c r="V13">
-        <v>4</v>
-      </c>
-      <c r="W13" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <v>4</v>
-      </c>
-      <c r="E14">
-        <v>3</v>
-      </c>
-      <c r="F14">
-        <v>3</v>
-      </c>
-      <c r="G14">
-        <v>3</v>
-      </c>
-      <c r="H14">
-        <v>-5</v>
-      </c>
-      <c r="I14">
-        <v>7</v>
-      </c>
-      <c r="J14">
-        <v>8</v>
-      </c>
-      <c r="K14">
-        <v>16</v>
-      </c>
-      <c r="L14">
-        <v>9</v>
-      </c>
-      <c r="M14">
-        <v>2</v>
-      </c>
-      <c r="N14">
-        <v>4</v>
-      </c>
-      <c r="O14">
-        <v>5</v>
-      </c>
-      <c r="P14">
-        <v>2</v>
-      </c>
-      <c r="Q14">
-        <v>5</v>
-      </c>
-      <c r="R14">
-        <v>3</v>
-      </c>
-      <c r="S14">
-        <v>5</v>
-      </c>
-      <c r="T14">
-        <v>4</v>
-      </c>
-      <c r="U14">
-        <v>2</v>
-      </c>
-      <c r="V14">
-        <v>4</v>
-      </c>
-      <c r="W14" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15">
-        <v>2</v>
-      </c>
-      <c r="D15">
-        <v>4</v>
-      </c>
-      <c r="E15">
-        <v>3</v>
-      </c>
-      <c r="F15">
-        <v>3</v>
-      </c>
-      <c r="G15">
-        <v>2</v>
-      </c>
-      <c r="H15">
-        <v>-1</v>
-      </c>
-      <c r="I15">
-        <v>-2</v>
-      </c>
-      <c r="J15">
-        <v>1</v>
-      </c>
-      <c r="K15">
-        <v>16</v>
-      </c>
-      <c r="L15">
-        <v>11</v>
-      </c>
-      <c r="M15">
-        <v>0</v>
-      </c>
-      <c r="N15">
-        <v>3</v>
-      </c>
-      <c r="O15">
-        <v>2</v>
-      </c>
-      <c r="P15">
-        <v>3</v>
-      </c>
-      <c r="Q15">
-        <v>3</v>
-      </c>
-      <c r="R15">
-        <v>1</v>
-      </c>
-      <c r="S15">
-        <v>3</v>
-      </c>
-      <c r="T15">
-        <v>2</v>
-      </c>
-      <c r="U15">
-        <v>3</v>
-      </c>
-      <c r="V15">
-        <v>3</v>
-      </c>
-      <c r="W15" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>2</v>
-      </c>
-      <c r="C16">
-        <v>5</v>
-      </c>
-      <c r="D16">
-        <v>3</v>
-      </c>
-      <c r="E16">
-        <v>3</v>
-      </c>
-      <c r="F16">
-        <v>-1</v>
-      </c>
-      <c r="G16">
-        <v>2</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <v>3</v>
-      </c>
-      <c r="J16">
-        <v>5</v>
-      </c>
-      <c r="K16">
-        <v>18</v>
-      </c>
-      <c r="L16">
-        <v>4</v>
-      </c>
-      <c r="M16">
-        <v>6</v>
-      </c>
-      <c r="N16">
-        <v>5</v>
-      </c>
-      <c r="O16">
-        <v>5</v>
-      </c>
-      <c r="P16">
-        <v>1</v>
-      </c>
-      <c r="Q16">
-        <v>5</v>
-      </c>
-      <c r="R16">
-        <v>2</v>
-      </c>
-      <c r="S16">
-        <v>5</v>
-      </c>
-      <c r="T16">
-        <v>5</v>
-      </c>
-      <c r="U16">
-        <v>1</v>
-      </c>
-      <c r="V16">
-        <v>5</v>
-      </c>
-      <c r="W16" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17">
-        <v>5</v>
-      </c>
-      <c r="D17">
-        <v>3</v>
-      </c>
-      <c r="E17">
-        <v>4</v>
-      </c>
-      <c r="F17">
-        <v>3</v>
-      </c>
-      <c r="G17">
-        <v>5</v>
-      </c>
-      <c r="H17">
-        <v>3</v>
-      </c>
-      <c r="I17">
-        <v>-1</v>
-      </c>
-      <c r="J17">
-        <v>8</v>
-      </c>
-      <c r="K17">
-        <v>17</v>
-      </c>
-      <c r="L17">
-        <v>5</v>
-      </c>
-      <c r="M17">
-        <v>10</v>
-      </c>
-      <c r="N17">
-        <v>5</v>
-      </c>
-      <c r="O17">
-        <v>4</v>
-      </c>
-      <c r="P17">
-        <v>1</v>
-      </c>
-      <c r="Q17">
-        <v>5</v>
-      </c>
-      <c r="R17">
-        <v>10</v>
-      </c>
-      <c r="S17">
-        <v>5</v>
-      </c>
-      <c r="T17">
-        <v>5</v>
-      </c>
-      <c r="U17">
-        <v>1</v>
-      </c>
-      <c r="V17">
-        <v>5</v>
-      </c>
-      <c r="W17" s="3">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>